<commit_message>
Lots of ML modeling
</commit_message>
<xml_diff>
--- a/Kip/data/corrFMAcqFMac.xlsx
+++ b/Kip/data/corrFMAcqFMac.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kip Madden\Desktop\dataScience\Project3\Kip\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{54F95FE3-9894-4294-98FF-0821E38AD59E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD4BA67-9A92-49FD-8A9C-61D5321CC544}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33214" yWindow="2271" windowWidth="30772" windowHeight="13252"/>
+    <workbookView xWindow="36626" yWindow="2169" windowWidth="24685" windowHeight="13148" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="corrFMAcqFMac" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">corrFMAcqFMac!$B$1:$R$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">corrFMAcqFMac!$A$1:$R$17</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
@@ -689,27 +689,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color theme="0"/>
@@ -1079,11 +1059,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A13" sqref="A13:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.5"/>
@@ -1208,58 +1188,58 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2">
-        <v>-2.7783873303340202E-4</v>
+        <v>-1.4852448341838399E-4</v>
       </c>
       <c r="D3" s="2">
-        <v>-6.8070941732721602E-3</v>
+        <v>-1.9159710407824701E-2</v>
       </c>
       <c r="E3" s="2">
-        <v>-0.38783056807012101</v>
+        <v>-0.38404584976137501</v>
       </c>
       <c r="F3" s="2">
-        <v>0.17886057553773799</v>
+        <v>0.19561240174092001</v>
       </c>
       <c r="G3" s="2">
-        <v>-0.15972460391618101</v>
+        <v>-0.15297015023375901</v>
       </c>
       <c r="H3" s="2">
-        <v>-0.12733109898449799</v>
+        <v>-0.12010966467909399</v>
       </c>
       <c r="I3" s="2">
-        <v>8.8277647441254298E-3</v>
+        <v>0.179342673117802</v>
       </c>
       <c r="J3" s="2">
-        <v>-0.20162514534024001</v>
+        <v>-0.208253390237126</v>
       </c>
       <c r="K3" s="2">
-        <v>0.96217852224509404</v>
+        <v>0.95186912154725001</v>
       </c>
       <c r="L3" s="2">
-        <v>0.14111015999342799</v>
+        <v>0.14763364775784801</v>
       </c>
       <c r="M3" s="2">
-        <v>5.4385114717743599E-2</v>
+        <v>5.1354668805340502E-2</v>
       </c>
       <c r="N3" s="2">
-        <v>-7.9050674769346393E-2</v>
+        <v>-7.5897959467574994E-2</v>
       </c>
       <c r="O3" s="2">
-        <v>-7.0425603754954394E-2</v>
+        <v>-6.8148661187687906E-2</v>
       </c>
       <c r="P3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="2">
         <v>0.924366713764318</v>
       </c>
-      <c r="Q3" s="2">
-        <v>1</v>
-      </c>
       <c r="R3" s="2">
-        <v>0.98139194008246899</v>
+        <v>0.98042085275520696</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.5">
@@ -1320,736 +1300,736 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>-1.89019744633169E-4</v>
+      </c>
+      <c r="E5" s="2">
+        <v>5.2457417061441201E-4</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2.79867866729532E-4</v>
+      </c>
+      <c r="G5" s="2">
+        <v>-3.27389015187829E-4</v>
+      </c>
+      <c r="H5" s="2">
+        <v>-3.4542058459296901E-4</v>
+      </c>
+      <c r="I5" s="2">
+        <v>2.8577798708081002E-4</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1.2214094676715899E-4</v>
+      </c>
+      <c r="K5" s="2">
+        <v>-1.36719878768663E-4</v>
+      </c>
+      <c r="L5" s="2">
+        <v>4.1157499830998698E-4</v>
+      </c>
+      <c r="M5" s="2">
+        <v>3.0353191579601102E-4</v>
+      </c>
+      <c r="N5" s="2">
+        <v>3.9300598152099901E-4</v>
+      </c>
+      <c r="O5" s="2">
+        <v>2.3706003016693201E-4</v>
+      </c>
+      <c r="P5" s="2">
         <v>-1.4852448341838399E-4</v>
       </c>
-      <c r="D5" s="2">
-        <v>-1.9159710407824701E-2</v>
-      </c>
-      <c r="E5" s="2">
-        <v>-0.38404584976137501</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.19561240174092001</v>
-      </c>
-      <c r="G5" s="2">
-        <v>-0.15297015023375901</v>
-      </c>
-      <c r="H5" s="2">
-        <v>-0.12010966467909399</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0.179342673117802</v>
-      </c>
-      <c r="J5" s="2">
-        <v>-0.208253390237126</v>
-      </c>
-      <c r="K5" s="2">
-        <v>0.95186912154725001</v>
-      </c>
-      <c r="L5" s="2">
-        <v>0.14763364775784801</v>
-      </c>
-      <c r="M5" s="2">
-        <v>5.1354668805340502E-2</v>
-      </c>
-      <c r="N5" s="2">
-        <v>-7.5897959467574994E-2</v>
-      </c>
-      <c r="O5" s="2">
-        <v>-6.8148661187687906E-2</v>
-      </c>
-      <c r="P5" s="2">
-        <v>1</v>
-      </c>
       <c r="Q5" s="2">
-        <v>0.924366713764318</v>
+        <v>-2.7783873303340202E-4</v>
       </c>
       <c r="R5" s="2">
-        <v>0.98042085275520696</v>
+        <v>-2.1816004980534901E-4</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.5">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
+      <c r="A6" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2">
-        <v>2.79867866729532E-4</v>
+        <v>4.1157499830998698E-4</v>
       </c>
       <c r="D6" s="2">
-        <v>5.80753579452341E-2</v>
+        <v>2.7200352666918701E-2</v>
       </c>
       <c r="E6" s="2">
-        <v>-0.35788648168558101</v>
+        <v>-0.11425123502886</v>
       </c>
       <c r="F6" s="2">
+        <v>0.102923022651534</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.124587296842431</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.13884678800890199</v>
+      </c>
+      <c r="I6" s="2">
+        <v>4.7761872206744597E-2</v>
+      </c>
+      <c r="J6" s="2">
+        <v>-0.123602702298135</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.14497241019396301</v>
+      </c>
+      <c r="L6" s="2">
         <v>1</v>
       </c>
-      <c r="G6" s="2">
-        <v>-4.3212985394627699E-3</v>
-      </c>
-      <c r="H6" s="2">
-        <v>4.2201690290334201E-2</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0.13547160508506401</v>
-      </c>
-      <c r="J6" s="2">
-        <v>7.1164692596257503E-2</v>
-      </c>
-      <c r="K6" s="2">
-        <v>0.183496635559005</v>
-      </c>
-      <c r="L6" s="2">
-        <v>0.102923022651534</v>
-      </c>
       <c r="M6" s="2">
-        <v>0.14066123606671599</v>
+        <v>2.1315087691030399E-2</v>
       </c>
       <c r="N6" s="2">
-        <v>-6.99710114737188E-2</v>
+        <v>0.164887804574639</v>
       </c>
       <c r="O6" s="2">
-        <v>-5.5620371257665897E-2</v>
+        <v>0.16322307053117799</v>
       </c>
       <c r="P6" s="2">
-        <v>0.19561240174092001</v>
+        <v>0.14763364775784801</v>
       </c>
       <c r="Q6" s="2">
-        <v>0.17886057553773799</v>
+        <v>0.14111015999342799</v>
       </c>
       <c r="R6" s="2">
-        <v>0.19077236481381399</v>
+        <v>0.147139344897042</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.5">
-      <c r="A7" s="5" t="s">
-        <v>21</v>
+      <c r="A7" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2">
-        <v>4.1157499830998698E-4</v>
+        <v>2.3706003016693201E-4</v>
       </c>
       <c r="D7" s="2">
-        <v>2.7200352666918701E-2</v>
+        <v>9.7118426749866291E-3</v>
       </c>
       <c r="E7" s="2">
-        <v>-0.11425123502886</v>
+        <v>6.9704058403688707E-2</v>
       </c>
       <c r="F7" s="2">
-        <v>0.102923022651534</v>
+        <v>-5.5620371257665897E-2</v>
       </c>
       <c r="G7" s="2">
-        <v>0.124587296842431</v>
+        <v>0.44517887941225498</v>
       </c>
       <c r="H7" s="2">
-        <v>0.13884678800890199</v>
+        <v>0.40053035313638002</v>
       </c>
       <c r="I7" s="2">
-        <v>4.7761872206744597E-2</v>
+        <v>-1.0759327890699199E-2</v>
       </c>
       <c r="J7" s="2">
-        <v>-0.123602702298135</v>
+        <v>4.2435325136155298E-2</v>
       </c>
       <c r="K7" s="2">
-        <v>0.14497241019396301</v>
+        <v>-6.8789600974356796E-2</v>
       </c>
       <c r="L7" s="2">
+        <v>0.16322307053117799</v>
+      </c>
+      <c r="M7" s="2">
+        <v>-3.4975459840884501E-2</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0.91333776475906503</v>
+      </c>
+      <c r="O7" s="2">
         <v>1</v>
       </c>
-      <c r="M7" s="2">
-        <v>2.1315087691030399E-2</v>
-      </c>
-      <c r="N7" s="2">
-        <v>0.164887804574639</v>
-      </c>
-      <c r="O7" s="2">
-        <v>0.16322307053117799</v>
-      </c>
       <c r="P7" s="2">
-        <v>0.14763364775784801</v>
+        <v>-6.8148661187687906E-2</v>
       </c>
       <c r="Q7" s="2">
-        <v>0.14111015999342799</v>
+        <v>-7.0425603754954394E-2</v>
       </c>
       <c r="R7" s="2">
-        <v>0.147139344897042</v>
+        <v>-7.0650001867426898E-2</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.5">
-      <c r="A8" s="6" t="s">
-        <v>22</v>
+      <c r="A8" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2">
-        <v>3.0353191579601102E-4</v>
+        <v>2.8577798708081002E-4</v>
       </c>
       <c r="D8" s="2">
-        <v>2.0846119238803602E-2</v>
+        <v>9.5470691379320096E-3</v>
       </c>
       <c r="E8" s="2">
-        <v>-6.9165957311247195E-2</v>
+        <v>2.9651557404021901E-2</v>
       </c>
       <c r="F8" s="2">
-        <v>0.14066123606671599</v>
+        <v>0.13547160508506401</v>
       </c>
       <c r="G8" s="2">
-        <v>-6.1956687759934702E-2</v>
+        <v>-2.2295583416363802E-3</v>
       </c>
       <c r="H8" s="2">
-        <v>-6.0262764073476499E-2</v>
+        <v>6.5512020232736399E-3</v>
       </c>
       <c r="I8" s="2">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2">
+        <v>-0.13994571978110901</v>
+      </c>
+      <c r="K8" s="2">
+        <v>8.2539705467966906E-2</v>
+      </c>
+      <c r="L8" s="2">
+        <v>4.7761872206744597E-2</v>
+      </c>
+      <c r="M8" s="2">
         <v>2.75181511014954E-2</v>
       </c>
-      <c r="J8" s="2">
-        <v>1.6723725302825301E-2</v>
-      </c>
-      <c r="K8" s="2">
-        <v>5.4470785144998202E-2</v>
-      </c>
-      <c r="L8" s="2">
-        <v>2.1315087691030399E-2</v>
-      </c>
-      <c r="M8" s="2">
-        <v>1</v>
-      </c>
       <c r="N8" s="2">
-        <v>-3.4366581281707699E-2</v>
+        <v>-4.9472496846017198E-3</v>
       </c>
       <c r="O8" s="2">
-        <v>-3.4975459840884501E-2</v>
+        <v>-1.0759327890699199E-2</v>
       </c>
       <c r="P8" s="2">
-        <v>5.1354668805340502E-2</v>
+        <v>0.179342673117802</v>
       </c>
       <c r="Q8" s="2">
-        <v>5.4385114717743599E-2</v>
+        <v>8.8277647441254298E-3</v>
       </c>
       <c r="R8" s="2">
-        <v>5.39181368174678E-2</v>
+        <v>9.4821358721567398E-2</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2">
+        <v>-1.89019744633169E-4</v>
+      </c>
+      <c r="D9" s="2">
         <v>1</v>
       </c>
-      <c r="D9" s="2">
-        <v>-1.89019744633169E-4</v>
-      </c>
       <c r="E9" s="2">
-        <v>5.2457417061441201E-4</v>
+        <v>5.4401133356633699E-2</v>
       </c>
       <c r="F9" s="2">
-        <v>2.79867866729532E-4</v>
+        <v>5.80753579452341E-2</v>
       </c>
       <c r="G9" s="2">
-        <v>-3.27389015187829E-4</v>
+        <v>4.2179565202098597E-2</v>
       </c>
       <c r="H9" s="2">
-        <v>-3.4542058459296901E-4</v>
+        <v>3.4010661760856098E-2</v>
       </c>
       <c r="I9" s="2">
-        <v>2.8577798708081002E-4</v>
+        <v>9.5470691379320096E-3</v>
       </c>
       <c r="J9" s="2">
-        <v>1.2214094676715899E-4</v>
+        <v>3.7765854603112402E-2</v>
       </c>
       <c r="K9" s="2">
-        <v>-1.36719878768663E-4</v>
+        <v>-1.3443991428868001E-2</v>
       </c>
       <c r="L9" s="2">
-        <v>4.1157499830998698E-4</v>
+        <v>2.7200352666918701E-2</v>
       </c>
       <c r="M9" s="2">
-        <v>3.0353191579601102E-4</v>
+        <v>2.0846119238803602E-2</v>
       </c>
       <c r="N9" s="2">
-        <v>3.9300598152099901E-4</v>
+        <v>1.5228865167264899E-2</v>
       </c>
       <c r="O9" s="2">
-        <v>2.3706003016693201E-4</v>
+        <v>9.7118426749866291E-3</v>
       </c>
       <c r="P9" s="2">
-        <v>-1.4852448341838399E-4</v>
+        <v>-1.9159710407824701E-2</v>
       </c>
       <c r="Q9" s="2">
-        <v>-2.7783873303340202E-4</v>
+        <v>-6.8070941732721602E-3</v>
       </c>
       <c r="R9" s="2">
-        <v>-2.1816004980534901E-4</v>
+        <v>-1.31567449523349E-2</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="2">
-        <v>2.8577798708081002E-4</v>
+        <v>-3.4542058459296901E-4</v>
       </c>
       <c r="D10" s="2">
-        <v>9.5470691379320096E-3</v>
+        <v>3.4010661760856098E-2</v>
       </c>
       <c r="E10" s="2">
-        <v>2.9651557404021901E-2</v>
+        <v>3.0677448378464402E-2</v>
       </c>
       <c r="F10" s="2">
-        <v>0.13547160508506401</v>
+        <v>4.2201690290334201E-2</v>
       </c>
       <c r="G10" s="2">
-        <v>-2.2295583416363802E-3</v>
+        <v>0.91747034157116503</v>
       </c>
       <c r="H10" s="2">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2">
         <v>6.5512020232736399E-3</v>
       </c>
-      <c r="I10" s="2">
-        <v>1</v>
-      </c>
       <c r="J10" s="2">
-        <v>-0.13994571978110901</v>
+        <v>7.9771956635613206E-2</v>
       </c>
       <c r="K10" s="2">
-        <v>8.2539705467966906E-2</v>
+        <v>-0.12406691443827</v>
       </c>
       <c r="L10" s="2">
-        <v>4.7761872206744597E-2</v>
+        <v>0.13884678800890199</v>
       </c>
       <c r="M10" s="2">
-        <v>2.75181511014954E-2</v>
+        <v>-6.0262764073476499E-2</v>
       </c>
       <c r="N10" s="2">
-        <v>-4.9472496846017198E-3</v>
+        <v>0.41396722823898102</v>
       </c>
       <c r="O10" s="2">
-        <v>-1.0759327890699199E-2</v>
+        <v>0.40053035313638002</v>
       </c>
       <c r="P10" s="2">
-        <v>0.179342673117802</v>
+        <v>-0.12010966467909399</v>
       </c>
       <c r="Q10" s="2">
-        <v>8.8277647441254298E-3</v>
+        <v>-0.12733109898449799</v>
       </c>
       <c r="R10" s="2">
-        <v>9.4821358721567398E-2</v>
+        <v>-0.12617420513608801</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C11" s="2">
-        <v>-3.4542058459296901E-4</v>
+        <v>1.2214094676715899E-4</v>
       </c>
       <c r="D11" s="2">
-        <v>3.4010661760856098E-2</v>
+        <v>3.7765854603112402E-2</v>
       </c>
       <c r="E11" s="2">
-        <v>3.0677448378464402E-2</v>
+        <v>9.6950852636375401E-2</v>
       </c>
       <c r="F11" s="2">
-        <v>4.2201690290334201E-2</v>
+        <v>7.1164692596257503E-2</v>
       </c>
       <c r="G11" s="2">
-        <v>0.91747034157116503</v>
+        <v>8.5448776884357397E-2</v>
       </c>
       <c r="H11" s="2">
+        <v>7.9771956635613206E-2</v>
+      </c>
+      <c r="I11" s="2">
+        <v>-0.13994571978110901</v>
+      </c>
+      <c r="J11" s="2">
         <v>1</v>
       </c>
-      <c r="I11" s="2">
-        <v>6.5512020232736399E-3</v>
-      </c>
-      <c r="J11" s="2">
-        <v>7.9771956635613206E-2</v>
-      </c>
       <c r="K11" s="2">
-        <v>-0.12406691443827</v>
+        <v>-0.20588339322032001</v>
       </c>
       <c r="L11" s="2">
-        <v>0.13884678800890199</v>
+        <v>-0.123602702298135</v>
       </c>
       <c r="M11" s="2">
-        <v>-6.0262764073476499E-2</v>
+        <v>1.6723725302825301E-2</v>
       </c>
       <c r="N11" s="2">
-        <v>0.41396722823898102</v>
+        <v>4.0236426925203399E-2</v>
       </c>
       <c r="O11" s="2">
-        <v>0.40053035313638002</v>
+        <v>4.2435325136155298E-2</v>
       </c>
       <c r="P11" s="2">
-        <v>-0.12010966467909399</v>
+        <v>-0.208253390237126</v>
       </c>
       <c r="Q11" s="2">
-        <v>-0.12733109898449799</v>
+        <v>-0.20162514534024001</v>
       </c>
       <c r="R11" s="2">
-        <v>-0.12617420513608801</v>
+        <v>-0.20888461119555901</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2">
+        <v>5.2457417061441201E-4</v>
+      </c>
+      <c r="D12" s="2">
+        <v>5.4401133356633699E-2</v>
+      </c>
+      <c r="E12" s="2">
         <v>1</v>
       </c>
-      <c r="C12" s="2">
-        <v>-1.89019744633169E-4</v>
-      </c>
-      <c r="D12" s="2">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2">
-        <v>5.4401133356633699E-2</v>
-      </c>
       <c r="F12" s="2">
-        <v>5.80753579452341E-2</v>
+        <v>-0.35788648168558101</v>
       </c>
       <c r="G12" s="2">
-        <v>4.2179565202098597E-2</v>
+        <v>0.104284126302152</v>
       </c>
       <c r="H12" s="2">
-        <v>3.4010661760856098E-2</v>
+        <v>3.0677448378464402E-2</v>
       </c>
       <c r="I12" s="2">
-        <v>9.5470691379320096E-3</v>
+        <v>2.9651557404021901E-2</v>
       </c>
       <c r="J12" s="2">
-        <v>3.7765854603112402E-2</v>
+        <v>9.6950852636375401E-2</v>
       </c>
       <c r="K12" s="2">
-        <v>-1.3443991428868001E-2</v>
+        <v>-0.38632745117404099</v>
       </c>
       <c r="L12" s="2">
-        <v>2.7200352666918701E-2</v>
+        <v>-0.11425123502886</v>
       </c>
       <c r="M12" s="2">
-        <v>2.0846119238803602E-2</v>
+        <v>-6.9165957311247195E-2</v>
       </c>
       <c r="N12" s="2">
-        <v>1.5228865167264899E-2</v>
+        <v>8.0710385224705097E-2</v>
       </c>
       <c r="O12" s="2">
-        <v>9.7118426749866291E-3</v>
+        <v>6.9704058403688707E-2</v>
       </c>
       <c r="P12" s="2">
-        <v>-1.9159710407824701E-2</v>
+        <v>-0.38404584976137501</v>
       </c>
       <c r="Q12" s="2">
-        <v>-6.8070941732721602E-3</v>
+        <v>-0.38783056807012101</v>
       </c>
       <c r="R12" s="2">
-        <v>-1.31567449523349E-2</v>
+        <v>-0.39347243445440599</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C13" s="2">
-        <v>2.3706003016693201E-4</v>
+        <v>-3.27389015187829E-4</v>
       </c>
       <c r="D13" s="2">
-        <v>9.7118426749866291E-3</v>
+        <v>4.2179565202098597E-2</v>
       </c>
       <c r="E13" s="2">
-        <v>6.9704058403688707E-2</v>
+        <v>0.104284126302152</v>
       </c>
       <c r="F13" s="2">
-        <v>-5.5620371257665897E-2</v>
+        <v>-4.3212985394627699E-3</v>
       </c>
       <c r="G13" s="2">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.91747034157116503</v>
+      </c>
+      <c r="I13" s="2">
+        <v>-2.2295583416363802E-3</v>
+      </c>
+      <c r="J13" s="2">
+        <v>8.5448776884357397E-2</v>
+      </c>
+      <c r="K13" s="2">
+        <v>-0.156457328118702</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0.124587296842431</v>
+      </c>
+      <c r="M13" s="2">
+        <v>-6.1956687759934702E-2</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0.45926968804436502</v>
+      </c>
+      <c r="O13" s="2">
         <v>0.44517887941225498</v>
       </c>
-      <c r="H13" s="2">
-        <v>0.40053035313638002</v>
-      </c>
-      <c r="I13" s="2">
-        <v>-1.0759327890699199E-2</v>
-      </c>
-      <c r="J13" s="2">
-        <v>4.2435325136155298E-2</v>
-      </c>
-      <c r="K13" s="2">
-        <v>-6.8789600974356796E-2</v>
-      </c>
-      <c r="L13" s="2">
-        <v>0.16322307053117799</v>
-      </c>
-      <c r="M13" s="2">
-        <v>-3.4975459840884501E-2</v>
-      </c>
-      <c r="N13" s="2">
-        <v>0.91333776475906503</v>
-      </c>
-      <c r="O13" s="2">
-        <v>1</v>
-      </c>
       <c r="P13" s="2">
-        <v>-6.8148661187687906E-2</v>
+        <v>-0.15297015023375901</v>
       </c>
       <c r="Q13" s="2">
-        <v>-7.0425603754954394E-2</v>
+        <v>-0.15972460391618101</v>
       </c>
       <c r="R13" s="2">
-        <v>-7.0650001867426898E-2</v>
+        <v>-0.15943308827017499</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.5">
-      <c r="A14" s="1" t="s">
-        <v>27</v>
+      <c r="A14" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C14" s="2">
-        <v>3.9300598152099901E-4</v>
+        <v>2.79867866729532E-4</v>
       </c>
       <c r="D14" s="2">
-        <v>1.5228865167264899E-2</v>
+        <v>5.80753579452341E-2</v>
       </c>
       <c r="E14" s="2">
-        <v>8.0710385224705097E-2</v>
+        <v>-0.35788648168558101</v>
       </c>
       <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2">
+        <v>-4.3212985394627699E-3</v>
+      </c>
+      <c r="H14" s="2">
+        <v>4.2201690290334201E-2</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.13547160508506401</v>
+      </c>
+      <c r="J14" s="2">
+        <v>7.1164692596257503E-2</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.183496635559005</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0.102923022651534</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0.14066123606671599</v>
+      </c>
+      <c r="N14" s="2">
         <v>-6.99710114737188E-2</v>
       </c>
-      <c r="G14" s="2">
-        <v>0.45926968804436502</v>
-      </c>
-      <c r="H14" s="2">
-        <v>0.41396722823898102</v>
-      </c>
-      <c r="I14" s="2">
-        <v>-4.9472496846017198E-3</v>
-      </c>
-      <c r="J14" s="2">
-        <v>4.0236426925203399E-2</v>
-      </c>
-      <c r="K14" s="2">
-        <v>-7.6965236983719001E-2</v>
-      </c>
-      <c r="L14" s="2">
-        <v>0.164887804574639</v>
-      </c>
-      <c r="M14" s="2">
-        <v>-3.4366581281707699E-2</v>
-      </c>
-      <c r="N14" s="2">
-        <v>1</v>
-      </c>
       <c r="O14" s="2">
-        <v>0.91333776475906503</v>
+        <v>-5.5620371257665897E-2</v>
       </c>
       <c r="P14" s="2">
-        <v>-7.5897959467574994E-2</v>
+        <v>0.19561240174092001</v>
       </c>
       <c r="Q14" s="2">
-        <v>-7.9050674769346393E-2</v>
+        <v>0.17886057553773799</v>
       </c>
       <c r="R14" s="2">
-        <v>-7.9002122412039202E-2</v>
+        <v>0.19077236481381399</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C15" s="2">
-        <v>1.2214094676715899E-4</v>
+        <v>3.9300598152099901E-4</v>
       </c>
       <c r="D15" s="2">
-        <v>3.7765854603112402E-2</v>
+        <v>1.5228865167264899E-2</v>
       </c>
       <c r="E15" s="2">
-        <v>9.6950852636375401E-2</v>
+        <v>8.0710385224705097E-2</v>
       </c>
       <c r="F15" s="2">
-        <v>7.1164692596257503E-2</v>
+        <v>-6.99710114737188E-2</v>
       </c>
       <c r="G15" s="2">
-        <v>8.5448776884357397E-2</v>
+        <v>0.45926968804436502</v>
       </c>
       <c r="H15" s="2">
-        <v>7.9771956635613206E-2</v>
+        <v>0.41396722823898102</v>
       </c>
       <c r="I15" s="2">
-        <v>-0.13994571978110901</v>
+        <v>-4.9472496846017198E-3</v>
       </c>
       <c r="J15" s="2">
+        <v>4.0236426925203399E-2</v>
+      </c>
+      <c r="K15" s="2">
+        <v>-7.6965236983719001E-2</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0.164887804574639</v>
+      </c>
+      <c r="M15" s="2">
+        <v>-3.4366581281707699E-2</v>
+      </c>
+      <c r="N15" s="2">
         <v>1</v>
       </c>
-      <c r="K15" s="2">
-        <v>-0.20588339322032001</v>
-      </c>
-      <c r="L15" s="2">
-        <v>-0.123602702298135</v>
-      </c>
-      <c r="M15" s="2">
-        <v>1.6723725302825301E-2</v>
-      </c>
-      <c r="N15" s="2">
-        <v>4.0236426925203399E-2</v>
-      </c>
       <c r="O15" s="2">
-        <v>4.2435325136155298E-2</v>
+        <v>0.91333776475906503</v>
       </c>
       <c r="P15" s="2">
-        <v>-0.208253390237126</v>
+        <v>-7.5897959467574994E-2</v>
       </c>
       <c r="Q15" s="2">
-        <v>-0.20162514534024001</v>
+        <v>-7.9050674769346393E-2</v>
       </c>
       <c r="R15" s="2">
-        <v>-0.20888461119555901</v>
+        <v>-7.9002122412039202E-2</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>4</v>
+        <v>18</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="C16" s="2">
-        <v>-3.27389015187829E-4</v>
+        <v>-2.7783873303340202E-4</v>
       </c>
       <c r="D16" s="2">
-        <v>4.2179565202098597E-2</v>
+        <v>-6.8070941732721602E-3</v>
       </c>
       <c r="E16" s="2">
-        <v>0.104284126302152</v>
+        <v>-0.38783056807012101</v>
       </c>
       <c r="F16" s="2">
-        <v>-4.3212985394627699E-3</v>
+        <v>0.17886057553773799</v>
       </c>
       <c r="G16" s="2">
+        <v>-0.15972460391618101</v>
+      </c>
+      <c r="H16" s="2">
+        <v>-0.12733109898449799</v>
+      </c>
+      <c r="I16" s="2">
+        <v>8.8277647441254298E-3</v>
+      </c>
+      <c r="J16" s="2">
+        <v>-0.20162514534024001</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0.96217852224509404</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0.14111015999342799</v>
+      </c>
+      <c r="M16" s="2">
+        <v>5.4385114717743599E-2</v>
+      </c>
+      <c r="N16" s="2">
+        <v>-7.9050674769346393E-2</v>
+      </c>
+      <c r="O16" s="2">
+        <v>-7.0425603754954394E-2</v>
+      </c>
+      <c r="P16" s="2">
+        <v>0.924366713764318</v>
+      </c>
+      <c r="Q16" s="2">
         <v>1</v>
       </c>
-      <c r="H16" s="2">
-        <v>0.91747034157116503</v>
-      </c>
-      <c r="I16" s="2">
-        <v>-2.2295583416363802E-3</v>
-      </c>
-      <c r="J16" s="2">
-        <v>8.5448776884357397E-2</v>
-      </c>
-      <c r="K16" s="2">
-        <v>-0.156457328118702</v>
-      </c>
-      <c r="L16" s="2">
-        <v>0.124587296842431</v>
-      </c>
-      <c r="M16" s="2">
-        <v>-6.1956687759934702E-2</v>
-      </c>
-      <c r="N16" s="2">
-        <v>0.45926968804436502</v>
-      </c>
-      <c r="O16" s="2">
-        <v>0.44517887941225498</v>
-      </c>
-      <c r="P16" s="2">
-        <v>-0.15297015023375901</v>
-      </c>
-      <c r="Q16" s="2">
-        <v>-0.15972460391618101</v>
-      </c>
       <c r="R16" s="2">
-        <v>-0.15943308827017499</v>
+        <v>0.98139194008246899</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.5">
-      <c r="A17" s="1" t="s">
-        <v>30</v>
+      <c r="A17" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C17" s="2">
-        <v>5.2457417061441201E-4</v>
+        <v>3.0353191579601102E-4</v>
       </c>
       <c r="D17" s="2">
-        <v>5.4401133356633699E-2</v>
+        <v>2.0846119238803602E-2</v>
       </c>
       <c r="E17" s="2">
+        <v>-6.9165957311247195E-2</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.14066123606671599</v>
+      </c>
+      <c r="G17" s="2">
+        <v>-6.1956687759934702E-2</v>
+      </c>
+      <c r="H17" s="2">
+        <v>-6.0262764073476499E-2</v>
+      </c>
+      <c r="I17" s="2">
+        <v>2.75181511014954E-2</v>
+      </c>
+      <c r="J17" s="2">
+        <v>1.6723725302825301E-2</v>
+      </c>
+      <c r="K17" s="2">
+        <v>5.4470785144998202E-2</v>
+      </c>
+      <c r="L17" s="2">
+        <v>2.1315087691030399E-2</v>
+      </c>
+      <c r="M17" s="2">
         <v>1</v>
       </c>
-      <c r="F17" s="2">
-        <v>-0.35788648168558101</v>
-      </c>
-      <c r="G17" s="2">
-        <v>0.104284126302152</v>
-      </c>
-      <c r="H17" s="2">
-        <v>3.0677448378464402E-2</v>
-      </c>
-      <c r="I17" s="2">
-        <v>2.9651557404021901E-2</v>
-      </c>
-      <c r="J17" s="2">
-        <v>9.6950852636375401E-2</v>
-      </c>
-      <c r="K17" s="2">
-        <v>-0.38632745117404099</v>
-      </c>
-      <c r="L17" s="2">
-        <v>-0.11425123502886</v>
-      </c>
-      <c r="M17" s="2">
-        <v>-6.9165957311247195E-2</v>
-      </c>
       <c r="N17" s="2">
-        <v>8.0710385224705097E-2</v>
+        <v>-3.4366581281707699E-2</v>
       </c>
       <c r="O17" s="2">
-        <v>6.9704058403688707E-2</v>
+        <v>-3.4975459840884501E-2</v>
       </c>
       <c r="P17" s="2">
-        <v>-0.38404584976137501</v>
+        <v>5.1354668805340502E-2</v>
       </c>
       <c r="Q17" s="2">
-        <v>-0.38783056807012101</v>
+        <v>5.4385114717743599E-2</v>
       </c>
       <c r="R17" s="2">
-        <v>-0.39347243445440599</v>
+        <v>5.39181368174678E-2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:R17">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:R17">
-      <sortCondition ref="E1:E17"/>
+  <autoFilter ref="A1:R17" xr:uid="{56CCDFB1-A3AE-4CF6-B3D0-9D1FC20366DE}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R17">
+      <sortCondition ref="B1:B17"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="C2:R17">

</xml_diff>